<commit_message>
added readme, optimzied dataneuxes html, integrated aaron code
</commit_message>
<xml_diff>
--- a/backends/data/leaderboard.xlsx
+++ b/backends/data/leaderboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,15 +453,90 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>moose</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>76</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-03-10T15:18:54.271858</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>team omega</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B3" t="n">
         <v>75</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>2025-03-07T14:15:50.897662</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">test </t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>75</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-03-10T13:27:48.108708</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>66</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-03-10T14:53:48.905717</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>march 10</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>66</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-03-10T13:42:36.068089</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>elon i</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>63</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-03-10T14:12:41.020226</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
everything wokrs, looking to make it harder
</commit_message>
<xml_diff>
--- a/backends/data/leaderboard.xlsx
+++ b/backends/data/leaderboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,37 +453,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>moose</t>
+          <t>mach 26</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-03-10T15:18:54.271858</t>
+          <t>2025-03-26T14:18:11.866225</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>team omega</t>
+          <t>moose</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-03-07T14:15:50.897662</t>
+          <t>2025-03-10T15:18:54.271858</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">test </t>
+          <t>team omega</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -491,29 +491,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-03-10T13:27:48.108708</t>
+          <t>2025-03-07T14:15:50.897662</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test</t>
+          <t xml:space="preserve">test </t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-03-10T14:53:48.905717</t>
+          <t>2025-03-10T13:27:48.108708</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>march 10</t>
+          <t>test</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -521,22 +521,67 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-03-10T13:42:36.068089</t>
+          <t>2025-03-10T14:53:48.905717</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>march 10</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>66</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-03-10T13:42:36.068089</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>elon i</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" t="n">
         <v>63</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>2025-03-10T14:12:41.020226</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-03-24T16:23:32.990396</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test 25 -2</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-03-25T14:15:03.571652</t>
         </is>
       </c>
     </row>

</xml_diff>